<commit_message>
Added data validation and more verbose errors; need to fix tests for create upload with excel comparison
</commit_message>
<xml_diff>
--- a/castoredc_api/tests/test_import/data_files_for_import_tests/data_file_study_final_errors.xlsx
+++ b/castoredc_api/tests/test_import/data_files_for_import_tests/data_file_study_final_errors.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>a</t>
   </si>
@@ -31,12 +31,6 @@
     <t>e</t>
   </si>
   <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Error;Error;Error</t>
-  </si>
-  <si>
     <t>record_id</t>
   </si>
   <si>
@@ -67,19 +61,46 @@
     <t>his_family</t>
   </si>
   <si>
-    <t>33;Error</t>
-  </si>
-  <si>
-    <t>Error;18-03-2022</t>
-  </si>
-  <si>
     <t>5;02-03-2023</t>
   </si>
   <si>
-    <t>Error;Error</t>
-  </si>
-  <si>
-    <t>28;Error</t>
+    <t>Error: unprocessable date</t>
+  </si>
+  <si>
+    <t>Error: non-existent option</t>
+  </si>
+  <si>
+    <t>Error: non-existent option;Error: non-existent option;Error: non-existent option</t>
+  </si>
+  <si>
+    <t>Error: non-existent option;Error: non-existent option</t>
+  </si>
+  <si>
+    <t>Error: unprocessable datetime</t>
+  </si>
+  <si>
+    <t>Error: unprocessable time</t>
+  </si>
+  <si>
+    <t>Error: year out of bounds</t>
+  </si>
+  <si>
+    <t>Error: not a year</t>
+  </si>
+  <si>
+    <t>Error: not a number</t>
+  </si>
+  <si>
+    <t>Error: wrong number of arguments for field</t>
+  </si>
+  <si>
+    <t>33;Error: unprocessable date</t>
+  </si>
+  <si>
+    <t>28;Error: unprocessable date</t>
+  </si>
+  <si>
+    <t>Error:not a number;18-03-2022</t>
   </si>
 </sst>
 </file>
@@ -428,7 +449,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,34 +469,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -483,31 +504,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -515,31 +536,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -547,31 +568,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -579,31 +600,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -611,31 +632,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Error checking of record_id before start of import
</commit_message>
<xml_diff>
--- a/castoredc_api/tests/test_import/data_files_for_import_tests/data_file_study_final_errors.xlsx
+++ b/castoredc_api/tests/test_import/data_files_for_import_tests/data_file_study_final_errors.xlsx
@@ -14,22 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
   <si>
     <t>record_id</t>
   </si>
@@ -101,6 +86,9 @@
   </si>
   <si>
     <t>Error: not a number;18-03-2022</t>
+  </si>
+  <si>
+    <t>Error: record does not exist in study</t>
   </si>
 </sst>
 </file>
@@ -448,13 +436,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" style="1" bestFit="1" customWidth="1"/>
@@ -469,194 +457,194 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>